<commit_message>
Extended set of registers to 256; last register is flags register
</commit_message>
<xml_diff>
--- a/CPU Instruction Set.xlsx
+++ b/CPU Instruction Set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryculpan/kcpu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A6DEA7-A240-954F-86B2-8A27D603DAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7817AAD1-9BE7-6D47-9FC8-12A8C20ED832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{543B224C-FB50-BF4D-B2DD-F8D0409D28B5}"/>
+    <workbookView xWindow="42240" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{543B224C-FB50-BF4D-B2DD-F8D0409D28B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="76">
   <si>
     <t>Instruction</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>.byte</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>ST R1, [R2]</t>
   </si>
 </sst>
 </file>
@@ -623,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFE8DF5-2928-4843-8D63-F0A05392873B}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,7 +665,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
@@ -668,16 +674,16 @@
         <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>26</v>
@@ -686,16 +692,16 @@
         <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>27</v>
@@ -704,57 +710,57 @@
         <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>45</v>
@@ -769,10 +775,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>45</v>
@@ -787,84 +793,84 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
@@ -879,10 +885,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
@@ -897,46 +903,46 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>45</v>
@@ -951,28 +957,28 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>45</v>
@@ -987,84 +993,82 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="D28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>45</v>
@@ -1081,19 +1085,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>64</v>
@@ -1101,10 +1105,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>25</v>
@@ -1119,79 +1123,81 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F34" s="1" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="1"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F38" s="1"/>
     </row>
@@ -1204,7 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FAE4C7-51DC-7048-89EC-561656DEECC1}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added indirect addressing for LD; added push/pop, shl/shr
</commit_message>
<xml_diff>
--- a/CPU Instruction Set.xlsx
+++ b/CPU Instruction Set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryculpan/kcpu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7817AAD1-9BE7-6D47-9FC8-12A8C20ED832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0EF182-1ABC-7044-A158-325CDFD3B225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42240" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{543B224C-FB50-BF4D-B2DD-F8D0409D28B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="77">
   <si>
     <t>Instruction</t>
   </si>
@@ -206,18 +206,6 @@
     <t>0x61</t>
   </si>
   <si>
-    <t>PUSH $0xabcd</t>
-  </si>
-  <si>
-    <t>POP $0xabcd</t>
-  </si>
-  <si>
-    <t>0x62</t>
-  </si>
-  <si>
-    <t>0x63</t>
-  </si>
-  <si>
     <t>CALL label</t>
   </si>
   <si>
@@ -242,9 +230,6 @@
     <t>0x03</t>
   </si>
   <si>
-    <t>REG</t>
-  </si>
-  <si>
     <t>0x13</t>
   </si>
   <si>
@@ -267,6 +252,24 @@
   </si>
   <si>
     <t>ST R1, [R2]</t>
+  </si>
+  <si>
+    <t>0x80</t>
+  </si>
+  <si>
+    <t>0-15</t>
+  </si>
+  <si>
+    <t>0x81</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>SHL R1,  0-15</t>
+  </si>
+  <si>
+    <t>SHR R1,  0-15</t>
   </si>
 </sst>
 </file>
@@ -302,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -312,6 +315,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFE8DF5-2928-4843-8D63-F0A05392873B}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,9 +647,10 @@
     <col min="4" max="4" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="87.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,10 +667,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -681,7 +691,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -699,7 +709,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -717,12 +727,12 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>45</v>
@@ -735,15 +745,15 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>25</v>
@@ -751,11 +761,9 @@
       <c r="E6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -773,7 +781,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -791,7 +799,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -809,15 +817,15 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>25</v>
@@ -826,10 +834,10 @@
         <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -847,7 +855,7 @@
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -865,7 +873,7 @@
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1080,7 +1088,7 @@
         <v>25</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1100,106 +1108,105 @@
         <v>25</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>64</v>
+      <c r="C34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1222,25 +1229,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new operations; added single-stepping and debugging to CPU
</commit_message>
<xml_diff>
--- a/CPU Instruction Set.xlsx
+++ b/CPU Instruction Set.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harryculpan/kcpu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BCFCDD-31E1-7F4E-A850-57732E81B9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE26119-B21D-A944-8CE1-F406BADF7627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42240" yWindow="920" windowWidth="28040" windowHeight="17440" xr2:uid="{543B224C-FB50-BF4D-B2DD-F8D0409D28B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="87">
   <si>
     <t>Instruction</t>
   </si>
@@ -245,9 +245,6 @@
     <t>.const</t>
   </si>
   <si>
-    <t>.byte</t>
-  </si>
-  <si>
     <t>0x04</t>
   </si>
   <si>
@@ -288,6 +285,21 @@
   </si>
   <si>
     <t>0x14</t>
+  </si>
+  <si>
+    <t>OUT 0, R1</t>
+  </si>
+  <si>
+    <t>0x51</t>
+  </si>
+  <si>
+    <t>.origin</t>
+  </si>
+  <si>
+    <t>.db</t>
+  </si>
+  <si>
+    <t>NO_CODE</t>
   </si>
 </sst>
 </file>
@@ -651,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFE8DF5-2928-4843-8D63-F0A05392873B}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -688,7 +700,7 @@
         <v>59</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -710,121 +722,106 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>45</v>
@@ -839,10 +836,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>45</v>
@@ -857,104 +854,104 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="1"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>25</v>
@@ -969,10 +966,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
@@ -987,46 +984,46 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>45</v>
@@ -1041,28 +1038,28 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>45</v>
@@ -1077,190 +1074,234 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="C29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F39" s="1"/>
+      <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F41" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1269,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FAE4C7-51DC-7048-89EC-561656DEECC1}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1281,7 +1322,7 @@
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1289,19 +1330,30 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>